<commit_message>
Modificaciones en las plantillas existentes y nuevos reportes
</commit_message>
<xml_diff>
--- a/Template/Export/Sari_R1_119.xlsx
+++ b/Template/Export/Sari_R1_119.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Template\Export\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="120" windowWidth="15480" windowHeight="7305"/>
   </bookViews>
@@ -14,7 +19,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Hoja1!$A$1:$P$62</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -22,9 +27,6 @@
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Total</t>
-  </si>
-  <si>
-    <t>Total SARI</t>
   </si>
   <si>
     <t>Total Hospitalization</t>
@@ -46,6 +48,9 @@
   </si>
   <si>
     <t>Number of cases of SARI and % of hospitalizations SARI by Epidemiological Week</t>
+  </si>
+  <si>
+    <t>Number of SARI cases</t>
   </si>
 </sst>
 </file>
@@ -249,7 +254,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -276,9 +281,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -290,9 +292,19 @@
     <xf numFmtId="1" fontId="6" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="7" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -313,12 +325,13 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF4F81BD"/>
       <color rgb="FFFFFF66"/>
       <color rgb="FFFFCC00"/>
       <color rgb="FFFFFF00"/>
@@ -328,6 +341,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -335,7 +351,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="es-GT"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -372,21 +388,31 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="7.0066407615381993E-2"/>
+          <c:y val="0.17149268991978411"/>
+          <c:w val="0.85986718476923607"/>
+          <c:h val="0.66903055792724708"/>
+        </c:manualLayout>
+      </c:layout>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
+          <c:idx val="1"/>
+          <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja1!$B$7:$B$59</c:f>
+              <c:f>Hoja1!$C$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1 2 3 4 5 6 7 8 9 10 11 12 13 14 15 16 17 18 19 20 21 22 23 24 25 26 27 28 29 30 31 32 33 34 35 36 37 38 39 40 41 42 43 44 45 46 47 48 49 50 51 52 53</c:v>
+                  <c:v>Number of SARI cases</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -570,26 +596,235 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="97392128"/>
-        <c:axId val="89231872"/>
+        <c:axId val="-2047628944"/>
+        <c:axId val="-2047619696"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredBarSeries>
+              <c15:ser>
+                <c:idx val="0"/>
+                <c:order val="0"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Hoja1!$B$6</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>Epidemiological Week</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:invertIfNegative val="0"/>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Hoja1!$B$7:$B$59</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>0</c:formatCode>
+                      <c:ptCount val="53"/>
+                      <c:pt idx="0">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>2</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>3</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>4</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>5</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>6</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>7</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>8</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>9</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>10</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>11</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>12</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>13</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>14</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>15</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>16</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>17</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>18</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>19</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="20">
+                        <c:v>21</c:v>
+                      </c:pt>
+                      <c:pt idx="21">
+                        <c:v>22</c:v>
+                      </c:pt>
+                      <c:pt idx="22">
+                        <c:v>23</c:v>
+                      </c:pt>
+                      <c:pt idx="23">
+                        <c:v>24</c:v>
+                      </c:pt>
+                      <c:pt idx="24">
+                        <c:v>25</c:v>
+                      </c:pt>
+                      <c:pt idx="25">
+                        <c:v>26</c:v>
+                      </c:pt>
+                      <c:pt idx="26">
+                        <c:v>27</c:v>
+                      </c:pt>
+                      <c:pt idx="27">
+                        <c:v>28</c:v>
+                      </c:pt>
+                      <c:pt idx="28">
+                        <c:v>29</c:v>
+                      </c:pt>
+                      <c:pt idx="29">
+                        <c:v>30</c:v>
+                      </c:pt>
+                      <c:pt idx="30">
+                        <c:v>31</c:v>
+                      </c:pt>
+                      <c:pt idx="31">
+                        <c:v>32</c:v>
+                      </c:pt>
+                      <c:pt idx="32">
+                        <c:v>33</c:v>
+                      </c:pt>
+                      <c:pt idx="33">
+                        <c:v>34</c:v>
+                      </c:pt>
+                      <c:pt idx="34">
+                        <c:v>35</c:v>
+                      </c:pt>
+                      <c:pt idx="35">
+                        <c:v>36</c:v>
+                      </c:pt>
+                      <c:pt idx="36">
+                        <c:v>37</c:v>
+                      </c:pt>
+                      <c:pt idx="37">
+                        <c:v>38</c:v>
+                      </c:pt>
+                      <c:pt idx="38">
+                        <c:v>39</c:v>
+                      </c:pt>
+                      <c:pt idx="39">
+                        <c:v>40</c:v>
+                      </c:pt>
+                      <c:pt idx="40">
+                        <c:v>41</c:v>
+                      </c:pt>
+                      <c:pt idx="41">
+                        <c:v>42</c:v>
+                      </c:pt>
+                      <c:pt idx="42">
+                        <c:v>43</c:v>
+                      </c:pt>
+                      <c:pt idx="43">
+                        <c:v>44</c:v>
+                      </c:pt>
+                      <c:pt idx="44">
+                        <c:v>45</c:v>
+                      </c:pt>
+                      <c:pt idx="45">
+                        <c:v>46</c:v>
+                      </c:pt>
+                      <c:pt idx="46">
+                        <c:v>47</c:v>
+                      </c:pt>
+                      <c:pt idx="47">
+                        <c:v>48</c:v>
+                      </c:pt>
+                      <c:pt idx="48">
+                        <c:v>49</c:v>
+                      </c:pt>
+                      <c:pt idx="49">
+                        <c:v>50</c:v>
+                      </c:pt>
+                      <c:pt idx="50">
+                        <c:v>51</c:v>
+                      </c:pt>
+                      <c:pt idx="51">
+                        <c:v>52</c:v>
+                      </c:pt>
+                      <c:pt idx="52">
+                        <c:v>53</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+              </c15:ser>
+            </c15:filteredBarSeries>
+          </c:ext>
+        </c:extLst>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
+          <c:idx val="3"/>
+          <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja1!$B$7:$B$59</c:f>
+              <c:f>Hoja1!$E$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1 2 3 4 5 6 7 8 9 10 11 12 13 14 15 16 17 18 19 20 21 22 23 24 25 26 27 28 29 30 31 32 33 34 35 36 37 38 39 40 41 42 43 44 45 46 47 48 49 50 51 52 53</c:v>
+                  <c:v>%  Hospitalization</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="4F81BD"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
@@ -773,20 +1008,257 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="97393152"/>
-        <c:axId val="89232448"/>
+        <c:axId val="-2047615344"/>
+        <c:axId val="-2047618608"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="2"/>
+                <c:order val="2"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Hoja1!$D$6</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>Total Hospitalization</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:marker>
+                  <c:symbol val="none"/>
+                </c:marker>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Hoja1!$D$7:$D$59</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="53"/>
+                      <c:pt idx="0">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="20">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="21">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="22">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="23">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="24">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="25">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="26">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="27">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="28">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="29">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="30">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="31">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="32">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="33">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="34">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="35">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="36">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="37">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="38">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="39">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="40">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="41">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="42">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="43">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="44">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="45">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="46">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="47">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="48">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="49">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="50">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="51">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="52">
+                        <c:v>0</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+              </c15:ser>
+            </c15:filteredLineSeries>
+          </c:ext>
+        </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="97392128"/>
+        <c:axId val="-2047628944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja1!$B$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Epidemiological Week</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.42242024165009223"/>
+              <c:y val="0.90224119575414519"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:txPr>
+            <a:bodyPr/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1100"/>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="89231872"/>
+        <c:crossAx val="-2047619696"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -794,38 +1266,88 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="89231872"/>
+        <c:axId val="-2047619696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja1!$C$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Number of SARI cases</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:txPr>
+            <a:bodyPr/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1100"/>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="97392128"/>
+        <c:crossAx val="-2047628944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="89232448"/>
+        <c:axId val="-2047618608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="r"/>
+        <c:title>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja1!$E$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>%  Hospitalization</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:txPr>
+            <a:bodyPr/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1100"/>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="97393152"/>
+        <c:crossAx val="-2047615344"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="97393152"/>
+        <c:axId val="-2047615344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -834,7 +1356,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="89232448"/>
+        <c:crossAx val="-2047618608"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -842,6 +1364,20 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.31830807733560684"/>
+          <c:y val="0.94355311007810772"/>
+          <c:w val="0.36338373121262912"/>
+          <c:h val="4.8414761407836071E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -890,7 +1426,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -932,7 +1468,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -967,7 +1503,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1179,74 +1715,78 @@
   <dimension ref="B1:O60"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B1:B1048576"/>
+      <selection activeCell="B2" sqref="B2:O2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" customWidth="1"/>
-    <col min="4" max="4" width="14" style="1" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" customWidth="1"/>
+    <col min="1" max="1" width="4.28515625" customWidth="1"/>
+    <col min="2" max="2" width="15" style="18" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" style="18" customWidth="1"/>
+    <col min="4" max="4" width="14" style="19" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" style="18" customWidth="1"/>
     <col min="6" max="15" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
-      <c r="L1" s="21"/>
-      <c r="M1" s="21"/>
-      <c r="N1" s="21"/>
-      <c r="O1" s="21"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
+      <c r="N1" s="22"/>
+      <c r="O1" s="22"/>
     </row>
     <row r="2" spans="2:15" ht="21" x14ac:dyDescent="0.35">
-      <c r="B2" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="23"/>
-      <c r="J2" s="23"/>
-      <c r="K2" s="23"/>
-      <c r="L2" s="23"/>
-      <c r="M2" s="23"/>
-      <c r="N2" s="23"/>
-      <c r="O2" s="23"/>
+      <c r="B2" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="24"/>
+      <c r="K2" s="24"/>
+      <c r="L2" s="24"/>
+      <c r="M2" s="24"/>
+      <c r="N2" s="24"/>
+      <c r="O2" s="24"/>
     </row>
     <row r="3" spans="2:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B3" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="H3" s="20"/>
-      <c r="I3" s="20"/>
+        <v>6</v>
+      </c>
+      <c r="C3"/>
+      <c r="D3" s="1"/>
+      <c r="E3"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B4" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19"/>
-      <c r="G4" s="19"/>
-      <c r="H4" s="19"/>
+      <c r="B4" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
       <c r="J4" s="2"/>
     </row>
     <row r="5" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -1257,16 +1797,16 @@
     </row>
     <row r="6" spans="2:15" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C6" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="E6" s="11" t="s">
         <v>2</v>
-      </c>
-      <c r="E6" s="12" t="s">
-        <v>3</v>
       </c>
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
@@ -1280,16 +1820,16 @@
       <c r="O6" s="8"/>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B7" s="17">
+      <c r="B7" s="16">
         <v>1</v>
       </c>
-      <c r="C7" s="16">
-        <v>0</v>
-      </c>
-      <c r="D7" s="16">
-        <v>0</v>
-      </c>
-      <c r="E7" s="18">
+      <c r="C7" s="17">
+        <v>0</v>
+      </c>
+      <c r="D7" s="17">
+        <v>0</v>
+      </c>
+      <c r="E7" s="15">
         <f t="shared" ref="E7:E58" si="0">IF(D7&lt;=0,0, C7*100/D7)</f>
         <v>0</v>
       </c>
@@ -1305,16 +1845,16 @@
       <c r="O7" s="9"/>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B8" s="17">
+      <c r="B8" s="16">
         <v>2</v>
       </c>
-      <c r="C8" s="16">
-        <v>0</v>
-      </c>
-      <c r="D8" s="16">
-        <v>0</v>
-      </c>
-      <c r="E8" s="18">
+      <c r="C8" s="17">
+        <v>0</v>
+      </c>
+      <c r="D8" s="17">
+        <v>0</v>
+      </c>
+      <c r="E8" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1330,16 +1870,16 @@
       <c r="O8" s="9"/>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B9" s="17">
+      <c r="B9" s="16">
         <v>3</v>
       </c>
-      <c r="C9" s="16">
-        <v>0</v>
-      </c>
-      <c r="D9" s="16">
-        <v>0</v>
-      </c>
-      <c r="E9" s="18">
+      <c r="C9" s="17">
+        <v>0</v>
+      </c>
+      <c r="D9" s="17">
+        <v>0</v>
+      </c>
+      <c r="E9" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1355,16 +1895,16 @@
       <c r="O9" s="9"/>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B10" s="17">
+      <c r="B10" s="16">
         <v>4</v>
       </c>
-      <c r="C10" s="16">
-        <v>0</v>
-      </c>
-      <c r="D10" s="16">
-        <v>0</v>
-      </c>
-      <c r="E10" s="18">
+      <c r="C10" s="17">
+        <v>0</v>
+      </c>
+      <c r="D10" s="17">
+        <v>0</v>
+      </c>
+      <c r="E10" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1380,16 +1920,16 @@
       <c r="O10" s="9"/>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B11" s="17">
+      <c r="B11" s="16">
         <v>5</v>
       </c>
-      <c r="C11" s="16">
-        <v>0</v>
-      </c>
-      <c r="D11" s="16">
-        <v>0</v>
-      </c>
-      <c r="E11" s="18">
+      <c r="C11" s="17">
+        <v>0</v>
+      </c>
+      <c r="D11" s="17">
+        <v>0</v>
+      </c>
+      <c r="E11" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1405,16 +1945,16 @@
       <c r="O11" s="9"/>
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B12" s="17">
+      <c r="B12" s="16">
         <v>6</v>
       </c>
-      <c r="C12" s="16">
-        <v>0</v>
-      </c>
-      <c r="D12" s="16">
-        <v>0</v>
-      </c>
-      <c r="E12" s="18">
+      <c r="C12" s="17">
+        <v>0</v>
+      </c>
+      <c r="D12" s="17">
+        <v>0</v>
+      </c>
+      <c r="E12" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1430,16 +1970,16 @@
       <c r="O12" s="9"/>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B13" s="17">
+      <c r="B13" s="16">
         <v>7</v>
       </c>
-      <c r="C13" s="16">
-        <v>0</v>
-      </c>
-      <c r="D13" s="16">
-        <v>0</v>
-      </c>
-      <c r="E13" s="18">
+      <c r="C13" s="17">
+        <v>0</v>
+      </c>
+      <c r="D13" s="17">
+        <v>0</v>
+      </c>
+      <c r="E13" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1455,16 +1995,16 @@
       <c r="O13" s="9"/>
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B14" s="17">
+      <c r="B14" s="16">
         <v>8</v>
       </c>
-      <c r="C14" s="16">
-        <v>0</v>
-      </c>
-      <c r="D14" s="16">
-        <v>0</v>
-      </c>
-      <c r="E14" s="18">
+      <c r="C14" s="17">
+        <v>0</v>
+      </c>
+      <c r="D14" s="17">
+        <v>0</v>
+      </c>
+      <c r="E14" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1480,16 +2020,16 @@
       <c r="O14" s="9"/>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B15" s="17">
+      <c r="B15" s="16">
         <v>9</v>
       </c>
-      <c r="C15" s="16">
-        <v>0</v>
-      </c>
-      <c r="D15" s="16">
-        <v>0</v>
-      </c>
-      <c r="E15" s="18">
+      <c r="C15" s="17">
+        <v>0</v>
+      </c>
+      <c r="D15" s="17">
+        <v>0</v>
+      </c>
+      <c r="E15" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1505,16 +2045,16 @@
       <c r="O15" s="9"/>
     </row>
     <row r="16" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B16" s="17">
+      <c r="B16" s="16">
         <v>10</v>
       </c>
-      <c r="C16" s="16">
-        <v>0</v>
-      </c>
-      <c r="D16" s="16">
-        <v>0</v>
-      </c>
-      <c r="E16" s="18">
+      <c r="C16" s="17">
+        <v>0</v>
+      </c>
+      <c r="D16" s="17">
+        <v>0</v>
+      </c>
+      <c r="E16" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1530,16 +2070,16 @@
       <c r="O16" s="9"/>
     </row>
     <row r="17" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B17" s="17">
+      <c r="B17" s="16">
         <v>11</v>
       </c>
-      <c r="C17" s="16">
-        <v>0</v>
-      </c>
-      <c r="D17" s="16">
-        <v>0</v>
-      </c>
-      <c r="E17" s="18">
+      <c r="C17" s="17">
+        <v>0</v>
+      </c>
+      <c r="D17" s="17">
+        <v>0</v>
+      </c>
+      <c r="E17" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1555,16 +2095,16 @@
       <c r="O17" s="9"/>
     </row>
     <row r="18" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B18" s="17">
+      <c r="B18" s="16">
         <v>12</v>
       </c>
-      <c r="C18" s="16">
-        <v>0</v>
-      </c>
-      <c r="D18" s="16">
-        <v>0</v>
-      </c>
-      <c r="E18" s="18">
+      <c r="C18" s="17">
+        <v>0</v>
+      </c>
+      <c r="D18" s="17">
+        <v>0</v>
+      </c>
+      <c r="E18" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1580,16 +2120,16 @@
       <c r="O18" s="9"/>
     </row>
     <row r="19" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B19" s="17">
+      <c r="B19" s="16">
         <v>13</v>
       </c>
-      <c r="C19" s="16">
-        <v>0</v>
-      </c>
-      <c r="D19" s="16">
-        <v>0</v>
-      </c>
-      <c r="E19" s="18">
+      <c r="C19" s="17">
+        <v>0</v>
+      </c>
+      <c r="D19" s="17">
+        <v>0</v>
+      </c>
+      <c r="E19" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1605,16 +2145,16 @@
       <c r="O19" s="9"/>
     </row>
     <row r="20" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B20" s="17">
+      <c r="B20" s="16">
         <v>14</v>
       </c>
-      <c r="C20" s="16">
-        <v>0</v>
-      </c>
-      <c r="D20" s="16">
-        <v>0</v>
-      </c>
-      <c r="E20" s="18">
+      <c r="C20" s="17">
+        <v>0</v>
+      </c>
+      <c r="D20" s="17">
+        <v>0</v>
+      </c>
+      <c r="E20" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1630,16 +2170,16 @@
       <c r="O20" s="9"/>
     </row>
     <row r="21" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B21" s="17">
+      <c r="B21" s="16">
         <v>15</v>
       </c>
-      <c r="C21" s="16">
-        <v>0</v>
-      </c>
-      <c r="D21" s="16">
-        <v>0</v>
-      </c>
-      <c r="E21" s="18">
+      <c r="C21" s="17">
+        <v>0</v>
+      </c>
+      <c r="D21" s="17">
+        <v>0</v>
+      </c>
+      <c r="E21" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1655,16 +2195,16 @@
       <c r="O21" s="9"/>
     </row>
     <row r="22" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B22" s="17">
+      <c r="B22" s="16">
         <v>16</v>
       </c>
-      <c r="C22" s="16">
-        <v>0</v>
-      </c>
-      <c r="D22" s="16">
-        <v>0</v>
-      </c>
-      <c r="E22" s="18">
+      <c r="C22" s="17">
+        <v>0</v>
+      </c>
+      <c r="D22" s="17">
+        <v>0</v>
+      </c>
+      <c r="E22" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1680,16 +2220,16 @@
       <c r="O22" s="9"/>
     </row>
     <row r="23" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B23" s="17">
+      <c r="B23" s="16">
         <v>17</v>
       </c>
-      <c r="C23" s="16">
-        <v>0</v>
-      </c>
-      <c r="D23" s="16">
-        <v>0</v>
-      </c>
-      <c r="E23" s="18">
+      <c r="C23" s="17">
+        <v>0</v>
+      </c>
+      <c r="D23" s="17">
+        <v>0</v>
+      </c>
+      <c r="E23" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1705,16 +2245,16 @@
       <c r="O23" s="9"/>
     </row>
     <row r="24" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B24" s="17">
+      <c r="B24" s="16">
         <v>18</v>
       </c>
-      <c r="C24" s="16">
-        <v>0</v>
-      </c>
-      <c r="D24" s="16">
-        <v>0</v>
-      </c>
-      <c r="E24" s="18">
+      <c r="C24" s="17">
+        <v>0</v>
+      </c>
+      <c r="D24" s="17">
+        <v>0</v>
+      </c>
+      <c r="E24" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1730,16 +2270,16 @@
       <c r="O24" s="9"/>
     </row>
     <row r="25" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B25" s="17">
+      <c r="B25" s="16">
         <v>19</v>
       </c>
-      <c r="C25" s="16">
-        <v>0</v>
-      </c>
-      <c r="D25" s="16">
-        <v>0</v>
-      </c>
-      <c r="E25" s="18">
+      <c r="C25" s="17">
+        <v>0</v>
+      </c>
+      <c r="D25" s="17">
+        <v>0</v>
+      </c>
+      <c r="E25" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1755,16 +2295,16 @@
       <c r="O25" s="9"/>
     </row>
     <row r="26" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B26" s="17">
+      <c r="B26" s="16">
         <v>20</v>
       </c>
-      <c r="C26" s="16">
-        <v>0</v>
-      </c>
-      <c r="D26" s="16">
-        <v>0</v>
-      </c>
-      <c r="E26" s="18">
+      <c r="C26" s="17">
+        <v>0</v>
+      </c>
+      <c r="D26" s="17">
+        <v>0</v>
+      </c>
+      <c r="E26" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1780,16 +2320,16 @@
       <c r="O26" s="9"/>
     </row>
     <row r="27" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B27" s="17">
+      <c r="B27" s="16">
         <v>21</v>
       </c>
-      <c r="C27" s="16">
-        <v>0</v>
-      </c>
-      <c r="D27" s="16">
-        <v>0</v>
-      </c>
-      <c r="E27" s="18">
+      <c r="C27" s="17">
+        <v>0</v>
+      </c>
+      <c r="D27" s="17">
+        <v>0</v>
+      </c>
+      <c r="E27" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1805,16 +2345,16 @@
       <c r="O27" s="9"/>
     </row>
     <row r="28" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B28" s="17">
+      <c r="B28" s="16">
         <v>22</v>
       </c>
-      <c r="C28" s="16">
-        <v>0</v>
-      </c>
-      <c r="D28" s="16">
-        <v>0</v>
-      </c>
-      <c r="E28" s="18">
+      <c r="C28" s="17">
+        <v>0</v>
+      </c>
+      <c r="D28" s="17">
+        <v>0</v>
+      </c>
+      <c r="E28" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1830,16 +2370,16 @@
       <c r="O28" s="9"/>
     </row>
     <row r="29" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B29" s="17">
+      <c r="B29" s="16">
         <v>23</v>
       </c>
-      <c r="C29" s="16">
-        <v>0</v>
-      </c>
-      <c r="D29" s="16">
-        <v>0</v>
-      </c>
-      <c r="E29" s="18">
+      <c r="C29" s="17">
+        <v>0</v>
+      </c>
+      <c r="D29" s="17">
+        <v>0</v>
+      </c>
+      <c r="E29" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1855,16 +2395,16 @@
       <c r="O29" s="9"/>
     </row>
     <row r="30" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B30" s="17">
+      <c r="B30" s="16">
         <v>24</v>
       </c>
-      <c r="C30" s="16">
-        <v>0</v>
-      </c>
-      <c r="D30" s="16">
-        <v>0</v>
-      </c>
-      <c r="E30" s="18">
+      <c r="C30" s="17">
+        <v>0</v>
+      </c>
+      <c r="D30" s="17">
+        <v>0</v>
+      </c>
+      <c r="E30" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1880,16 +2420,16 @@
       <c r="O30" s="9"/>
     </row>
     <row r="31" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B31" s="17">
+      <c r="B31" s="16">
         <v>25</v>
       </c>
-      <c r="C31" s="16">
-        <v>0</v>
-      </c>
-      <c r="D31" s="16">
-        <v>0</v>
-      </c>
-      <c r="E31" s="18">
+      <c r="C31" s="17">
+        <v>0</v>
+      </c>
+      <c r="D31" s="17">
+        <v>0</v>
+      </c>
+      <c r="E31" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1905,16 +2445,16 @@
       <c r="O31" s="9"/>
     </row>
     <row r="32" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B32" s="17">
+      <c r="B32" s="16">
         <v>26</v>
       </c>
-      <c r="C32" s="16">
-        <v>0</v>
-      </c>
-      <c r="D32" s="16">
-        <v>0</v>
-      </c>
-      <c r="E32" s="18">
+      <c r="C32" s="17">
+        <v>0</v>
+      </c>
+      <c r="D32" s="17">
+        <v>0</v>
+      </c>
+      <c r="E32" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1930,16 +2470,16 @@
       <c r="O32" s="9"/>
     </row>
     <row r="33" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B33" s="17">
+      <c r="B33" s="16">
         <v>27</v>
       </c>
-      <c r="C33" s="16">
-        <v>0</v>
-      </c>
-      <c r="D33" s="16">
-        <v>0</v>
-      </c>
-      <c r="E33" s="18">
+      <c r="C33" s="17">
+        <v>0</v>
+      </c>
+      <c r="D33" s="17">
+        <v>0</v>
+      </c>
+      <c r="E33" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1955,16 +2495,16 @@
       <c r="O33" s="9"/>
     </row>
     <row r="34" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B34" s="17">
+      <c r="B34" s="16">
         <v>28</v>
       </c>
-      <c r="C34" s="16">
-        <v>0</v>
-      </c>
-      <c r="D34" s="16">
-        <v>0</v>
-      </c>
-      <c r="E34" s="18">
+      <c r="C34" s="17">
+        <v>0</v>
+      </c>
+      <c r="D34" s="17">
+        <v>0</v>
+      </c>
+      <c r="E34" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1980,16 +2520,16 @@
       <c r="O34" s="9"/>
     </row>
     <row r="35" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B35" s="17">
+      <c r="B35" s="16">
         <v>29</v>
       </c>
-      <c r="C35" s="16">
-        <v>0</v>
-      </c>
-      <c r="D35" s="16">
-        <v>0</v>
-      </c>
-      <c r="E35" s="18">
+      <c r="C35" s="17">
+        <v>0</v>
+      </c>
+      <c r="D35" s="17">
+        <v>0</v>
+      </c>
+      <c r="E35" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2005,16 +2545,16 @@
       <c r="O35" s="9"/>
     </row>
     <row r="36" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B36" s="17">
+      <c r="B36" s="16">
         <v>30</v>
       </c>
-      <c r="C36" s="16">
-        <v>0</v>
-      </c>
-      <c r="D36" s="16">
-        <v>0</v>
-      </c>
-      <c r="E36" s="18">
+      <c r="C36" s="17">
+        <v>0</v>
+      </c>
+      <c r="D36" s="17">
+        <v>0</v>
+      </c>
+      <c r="E36" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2030,16 +2570,16 @@
       <c r="O36" s="9"/>
     </row>
     <row r="37" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B37" s="17">
+      <c r="B37" s="16">
         <v>31</v>
       </c>
-      <c r="C37" s="16">
-        <v>0</v>
-      </c>
-      <c r="D37" s="16">
-        <v>0</v>
-      </c>
-      <c r="E37" s="18">
+      <c r="C37" s="17">
+        <v>0</v>
+      </c>
+      <c r="D37" s="17">
+        <v>0</v>
+      </c>
+      <c r="E37" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2055,16 +2595,16 @@
       <c r="O37" s="9"/>
     </row>
     <row r="38" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B38" s="17">
+      <c r="B38" s="16">
         <v>32</v>
       </c>
-      <c r="C38" s="16">
-        <v>0</v>
-      </c>
-      <c r="D38" s="16">
-        <v>0</v>
-      </c>
-      <c r="E38" s="18">
+      <c r="C38" s="17">
+        <v>0</v>
+      </c>
+      <c r="D38" s="17">
+        <v>0</v>
+      </c>
+      <c r="E38" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2080,16 +2620,16 @@
       <c r="O38" s="9"/>
     </row>
     <row r="39" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B39" s="17">
+      <c r="B39" s="16">
         <v>33</v>
       </c>
-      <c r="C39" s="16">
-        <v>0</v>
-      </c>
-      <c r="D39" s="16">
-        <v>0</v>
-      </c>
-      <c r="E39" s="18">
+      <c r="C39" s="17">
+        <v>0</v>
+      </c>
+      <c r="D39" s="17">
+        <v>0</v>
+      </c>
+      <c r="E39" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2105,16 +2645,16 @@
       <c r="O39" s="9"/>
     </row>
     <row r="40" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B40" s="17">
+      <c r="B40" s="16">
         <v>34</v>
       </c>
-      <c r="C40" s="16">
-        <v>0</v>
-      </c>
-      <c r="D40" s="16">
-        <v>0</v>
-      </c>
-      <c r="E40" s="18">
+      <c r="C40" s="17">
+        <v>0</v>
+      </c>
+      <c r="D40" s="17">
+        <v>0</v>
+      </c>
+      <c r="E40" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2130,16 +2670,16 @@
       <c r="O40" s="9"/>
     </row>
     <row r="41" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B41" s="17">
+      <c r="B41" s="16">
         <v>35</v>
       </c>
-      <c r="C41" s="16">
-        <v>0</v>
-      </c>
-      <c r="D41" s="16">
-        <v>0</v>
-      </c>
-      <c r="E41" s="18">
+      <c r="C41" s="17">
+        <v>0</v>
+      </c>
+      <c r="D41" s="17">
+        <v>0</v>
+      </c>
+      <c r="E41" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2155,16 +2695,16 @@
       <c r="O41" s="9"/>
     </row>
     <row r="42" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B42" s="17">
+      <c r="B42" s="16">
         <v>36</v>
       </c>
-      <c r="C42" s="16">
-        <v>0</v>
-      </c>
-      <c r="D42" s="16">
-        <v>0</v>
-      </c>
-      <c r="E42" s="18">
+      <c r="C42" s="17">
+        <v>0</v>
+      </c>
+      <c r="D42" s="17">
+        <v>0</v>
+      </c>
+      <c r="E42" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2180,16 +2720,16 @@
       <c r="O42" s="9"/>
     </row>
     <row r="43" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B43" s="17">
+      <c r="B43" s="16">
         <v>37</v>
       </c>
-      <c r="C43" s="16">
-        <v>0</v>
-      </c>
-      <c r="D43" s="16">
-        <v>0</v>
-      </c>
-      <c r="E43" s="18">
+      <c r="C43" s="17">
+        <v>0</v>
+      </c>
+      <c r="D43" s="17">
+        <v>0</v>
+      </c>
+      <c r="E43" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2205,16 +2745,16 @@
       <c r="O43" s="9"/>
     </row>
     <row r="44" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B44" s="17">
+      <c r="B44" s="16">
         <v>38</v>
       </c>
-      <c r="C44" s="16">
-        <v>0</v>
-      </c>
-      <c r="D44" s="16">
-        <v>0</v>
-      </c>
-      <c r="E44" s="18">
+      <c r="C44" s="17">
+        <v>0</v>
+      </c>
+      <c r="D44" s="17">
+        <v>0</v>
+      </c>
+      <c r="E44" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2230,16 +2770,16 @@
       <c r="O44" s="9"/>
     </row>
     <row r="45" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B45" s="17">
+      <c r="B45" s="16">
         <v>39</v>
       </c>
-      <c r="C45" s="16">
-        <v>0</v>
-      </c>
-      <c r="D45" s="16">
-        <v>0</v>
-      </c>
-      <c r="E45" s="18">
+      <c r="C45" s="17">
+        <v>0</v>
+      </c>
+      <c r="D45" s="17">
+        <v>0</v>
+      </c>
+      <c r="E45" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2255,16 +2795,16 @@
       <c r="O45" s="9"/>
     </row>
     <row r="46" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B46" s="17">
+      <c r="B46" s="16">
         <v>40</v>
       </c>
-      <c r="C46" s="16">
-        <v>0</v>
-      </c>
-      <c r="D46" s="16">
-        <v>0</v>
-      </c>
-      <c r="E46" s="18">
+      <c r="C46" s="17">
+        <v>0</v>
+      </c>
+      <c r="D46" s="17">
+        <v>0</v>
+      </c>
+      <c r="E46" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2280,16 +2820,16 @@
       <c r="O46" s="9"/>
     </row>
     <row r="47" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B47" s="17">
+      <c r="B47" s="16">
         <v>41</v>
       </c>
-      <c r="C47" s="16">
-        <v>0</v>
-      </c>
-      <c r="D47" s="16">
-        <v>0</v>
-      </c>
-      <c r="E47" s="18">
+      <c r="C47" s="17">
+        <v>0</v>
+      </c>
+      <c r="D47" s="17">
+        <v>0</v>
+      </c>
+      <c r="E47" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2305,16 +2845,16 @@
       <c r="O47" s="9"/>
     </row>
     <row r="48" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B48" s="17">
+      <c r="B48" s="16">
         <v>42</v>
       </c>
-      <c r="C48" s="16">
-        <v>0</v>
-      </c>
-      <c r="D48" s="16">
-        <v>0</v>
-      </c>
-      <c r="E48" s="18">
+      <c r="C48" s="17">
+        <v>0</v>
+      </c>
+      <c r="D48" s="17">
+        <v>0</v>
+      </c>
+      <c r="E48" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2330,16 +2870,16 @@
       <c r="O48" s="9"/>
     </row>
     <row r="49" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B49" s="17">
+      <c r="B49" s="16">
         <v>43</v>
       </c>
-      <c r="C49" s="16">
-        <v>0</v>
-      </c>
-      <c r="D49" s="16">
-        <v>0</v>
-      </c>
-      <c r="E49" s="18">
+      <c r="C49" s="17">
+        <v>0</v>
+      </c>
+      <c r="D49" s="17">
+        <v>0</v>
+      </c>
+      <c r="E49" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2355,16 +2895,16 @@
       <c r="O49" s="9"/>
     </row>
     <row r="50" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B50" s="17">
+      <c r="B50" s="16">
         <v>44</v>
       </c>
-      <c r="C50" s="16">
-        <v>0</v>
-      </c>
-      <c r="D50" s="16">
-        <v>0</v>
-      </c>
-      <c r="E50" s="18">
+      <c r="C50" s="17">
+        <v>0</v>
+      </c>
+      <c r="D50" s="17">
+        <v>0</v>
+      </c>
+      <c r="E50" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2380,16 +2920,16 @@
       <c r="O50" s="9"/>
     </row>
     <row r="51" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B51" s="17">
+      <c r="B51" s="16">
         <v>45</v>
       </c>
-      <c r="C51" s="16">
-        <v>0</v>
-      </c>
-      <c r="D51" s="16">
-        <v>0</v>
-      </c>
-      <c r="E51" s="18">
+      <c r="C51" s="17">
+        <v>0</v>
+      </c>
+      <c r="D51" s="17">
+        <v>0</v>
+      </c>
+      <c r="E51" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2405,16 +2945,16 @@
       <c r="O51" s="9"/>
     </row>
     <row r="52" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B52" s="17">
+      <c r="B52" s="16">
         <v>46</v>
       </c>
-      <c r="C52" s="16">
-        <v>0</v>
-      </c>
-      <c r="D52" s="16">
-        <v>0</v>
-      </c>
-      <c r="E52" s="18">
+      <c r="C52" s="17">
+        <v>0</v>
+      </c>
+      <c r="D52" s="17">
+        <v>0</v>
+      </c>
+      <c r="E52" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2430,16 +2970,16 @@
       <c r="O52" s="9"/>
     </row>
     <row r="53" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B53" s="17">
+      <c r="B53" s="16">
         <v>47</v>
       </c>
-      <c r="C53" s="16">
-        <v>0</v>
-      </c>
-      <c r="D53" s="16">
-        <v>0</v>
-      </c>
-      <c r="E53" s="18">
+      <c r="C53" s="17">
+        <v>0</v>
+      </c>
+      <c r="D53" s="17">
+        <v>0</v>
+      </c>
+      <c r="E53" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2455,16 +2995,16 @@
       <c r="O53" s="9"/>
     </row>
     <row r="54" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B54" s="17">
+      <c r="B54" s="16">
         <v>48</v>
       </c>
-      <c r="C54" s="16">
-        <v>0</v>
-      </c>
-      <c r="D54" s="16">
-        <v>0</v>
-      </c>
-      <c r="E54" s="18">
+      <c r="C54" s="17">
+        <v>0</v>
+      </c>
+      <c r="D54" s="17">
+        <v>0</v>
+      </c>
+      <c r="E54" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2480,16 +3020,16 @@
       <c r="O54" s="9"/>
     </row>
     <row r="55" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B55" s="17">
+      <c r="B55" s="16">
         <v>49</v>
       </c>
-      <c r="C55" s="16">
-        <v>0</v>
-      </c>
-      <c r="D55" s="16">
-        <v>0</v>
-      </c>
-      <c r="E55" s="18">
+      <c r="C55" s="17">
+        <v>0</v>
+      </c>
+      <c r="D55" s="17">
+        <v>0</v>
+      </c>
+      <c r="E55" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2505,16 +3045,16 @@
       <c r="O55" s="9"/>
     </row>
     <row r="56" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B56" s="17">
+      <c r="B56" s="16">
         <v>50</v>
       </c>
-      <c r="C56" s="16">
-        <v>0</v>
-      </c>
-      <c r="D56" s="16">
-        <v>0</v>
-      </c>
-      <c r="E56" s="18">
+      <c r="C56" s="17">
+        <v>0</v>
+      </c>
+      <c r="D56" s="17">
+        <v>0</v>
+      </c>
+      <c r="E56" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2530,16 +3070,16 @@
       <c r="O56" s="9"/>
     </row>
     <row r="57" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B57" s="17">
+      <c r="B57" s="16">
         <v>51</v>
       </c>
-      <c r="C57" s="16">
-        <v>0</v>
-      </c>
-      <c r="D57" s="16">
-        <v>0</v>
-      </c>
-      <c r="E57" s="18">
+      <c r="C57" s="17">
+        <v>0</v>
+      </c>
+      <c r="D57" s="17">
+        <v>0</v>
+      </c>
+      <c r="E57" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2555,16 +3095,16 @@
       <c r="O57" s="9"/>
     </row>
     <row r="58" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B58" s="17">
+      <c r="B58" s="16">
         <v>52</v>
       </c>
-      <c r="C58" s="16">
-        <v>0</v>
-      </c>
-      <c r="D58" s="16">
-        <v>0</v>
-      </c>
-      <c r="E58" s="18">
+      <c r="C58" s="17">
+        <v>0</v>
+      </c>
+      <c r="D58" s="17">
+        <v>0</v>
+      </c>
+      <c r="E58" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2580,16 +3120,16 @@
       <c r="O58" s="9"/>
     </row>
     <row r="59" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B59" s="17">
+      <c r="B59" s="16">
         <v>53</v>
       </c>
-      <c r="C59" s="16">
-        <v>0</v>
-      </c>
-      <c r="D59" s="16">
-        <v>0</v>
-      </c>
-      <c r="E59" s="18">
+      <c r="C59" s="17">
+        <v>0</v>
+      </c>
+      <c r="D59" s="17">
+        <v>0</v>
+      </c>
+      <c r="E59" s="15">
         <f>IF(D59&lt;=0,0, C59*100/D59)</f>
         <v>0</v>
       </c>
@@ -2605,18 +3145,18 @@
       <c r="O59" s="9"/>
     </row>
     <row r="60" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B60" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="C60" s="14">
+      <c r="B60" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C60" s="13">
         <f>SUM(C7:C59)</f>
         <v>0</v>
       </c>
-      <c r="D60" s="14">
+      <c r="D60" s="13">
         <f>SUM(D7:D59)</f>
         <v>0</v>
       </c>
-      <c r="E60" s="15">
+      <c r="E60" s="14">
         <f>IF(C60=0,0,IF(D60=0,0,(D60/C60*100)))</f>
         <v>0</v>
       </c>
@@ -2653,7 +3193,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2665,7 +3205,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>